<commit_message>
Updated distances and RPM values as of beginning of matches
</commit_message>
<xml_diff>
--- a/DistanceVelocityPolynomial.xlsx
+++ b/DistanceVelocityPolynomial.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chriso\Documents\source\2022-Robot\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chris\Source\repos\2022-Robot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{604CACA1-C67D-4B52-91D9-CAE0A54B5BFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5E21617-AE7B-4D7E-B5DC-2C0FC97AD20D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13875" xr2:uid="{EEFDD230-E3A1-409D-A376-9E1A77C1EC02}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="21820" windowHeight="14620" activeTab="1" xr2:uid="{EEFDD230-E3A1-409D-A376-9E1A77C1EC02}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Saturday Practice" sheetId="1" r:id="rId1"/>
+    <sheet name="Jackson Comp" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="2">
   <si>
     <t>Distance in Inches</t>
   </si>
@@ -217,7 +218,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$11</c:f>
+              <c:f>'Saturday Practice'!$A$2:$A$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -256,7 +257,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$11</c:f>
+              <c:f>'Saturday Practice'!$B$2:$B$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -487,7 +488,507 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="3.7179528601280896E-2"/>
+          <c:y val="8.7778936392075083E-2"/>
+          <c:w val="0.93258883671969861"/>
+          <c:h val="0.87426847191546309"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="poly"/>
+            <c:order val="3"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.22413836589420366"/>
+                  <c:y val="-9.6605087825560265E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:pPr>
+                      <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                        <a:solidFill>
+                          <a:schemeClr val="tx1">
+                            <a:lumMod val="65000"/>
+                            <a:lumOff val="35000"/>
+                          </a:schemeClr>
+                        </a:solidFill>
+                        <a:latin typeface="+mn-lt"/>
+                        <a:ea typeface="+mn-ea"/>
+                        <a:cs typeface="+mn-cs"/>
+                      </a:defRPr>
+                    </a:pPr>
+                    <a:r>
+                      <a:rPr lang="en-US" sz="2800" baseline="0"/>
+                      <a:t>y = 0.0012x</a:t>
+                    </a:r>
+                    <a:r>
+                      <a:rPr lang="en-US" sz="2800" baseline="30000"/>
+                      <a:t>3</a:t>
+                    </a:r>
+                    <a:r>
+                      <a:rPr lang="en-US" sz="2800" baseline="0"/>
+                      <a:t> - 0.3501x</a:t>
+                    </a:r>
+                    <a:r>
+                      <a:rPr lang="en-US" sz="2800" baseline="30000"/>
+                      <a:t>2</a:t>
+                    </a:r>
+                    <a:r>
+                      <a:rPr lang="en-US" sz="2800" baseline="0"/>
+                      <a:t> + 45.719x + 1530.6</a:t>
+                    </a:r>
+                    <a:endParaRPr lang="en-US" sz="2800"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Jackson Comp'!$A$2:$A$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>63</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>81</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>88</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>103.6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>112</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>121</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>129</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>139.30000000000001</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>142.6</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>147.69999999999999</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>183</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Jackson Comp'!$B$2:$B$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>3300</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3650</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3720</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3900</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4020</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4060</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4200</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4510</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>4600</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>4700</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>5800</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-BCB0-4934-8B54-CE973F80FA1A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1363302495"/>
+        <c:axId val="1363301663"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1363302495"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="190"/>
+          <c:min val="50"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1363301663"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1363301663"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="6500"/>
+          <c:min val="2500"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1363302495"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -1043,6 +1544,522 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -1064,6 +2081,47 @@
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{843B4780-0FEA-4B50-A566-275BB2FC66DD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>120650</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>69850</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>82550</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{96C7A578-74F6-3055-1A18-0DA678AF1EF4}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1381,19 +2439,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20278FAF-F0D5-4B1B-A05C-6FE2675CF777}">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:B23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B23" sqref="A14:B23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.86328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.1328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.08984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1401,7 +2459,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>65.400000000000006</v>
       </c>
@@ -1409,7 +2467,7 @@
         <v>3450</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>72.55</v>
       </c>
@@ -1417,7 +2475,7 @@
         <v>3525</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>75.900000000000006</v>
       </c>
@@ -1425,7 +2483,7 @@
         <v>3600</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>94.1</v>
       </c>
@@ -1433,7 +2491,7 @@
         <v>3850</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>103.95</v>
       </c>
@@ -1441,7 +2499,7 @@
         <v>4050</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>115.9</v>
       </c>
@@ -1449,7 +2507,7 @@
         <v>4200</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>121.7</v>
       </c>
@@ -1457,7 +2515,7 @@
         <v>4220</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>129</v>
       </c>
@@ -1465,7 +2523,7 @@
         <v>4300</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>141.4</v>
       </c>
@@ -1473,12 +2531,184 @@
         <v>4750</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>149</v>
       </c>
       <c r="B11">
         <v>5400</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A14">
+        <v>63</v>
+      </c>
+      <c r="B14">
+        <v>3300</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A16">
+        <v>81</v>
+      </c>
+      <c r="B16">
+        <v>3650</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A17">
+        <v>112</v>
+      </c>
+      <c r="B17">
+        <v>3980</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A19">
+        <v>117.7</v>
+      </c>
+      <c r="B19">
+        <v>4205</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A20">
+        <v>119.4</v>
+      </c>
+      <c r="B20">
+        <v>4233</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A22">
+        <v>130</v>
+      </c>
+      <c r="B22">
+        <v>4340</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A23">
+        <v>142.6</v>
+      </c>
+      <c r="B23">
+        <v>4650</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0CE5BD1-6D64-45B1-ABA7-0B5F30DB1EA8}">
+  <dimension ref="A1:B14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="15.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.6328125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>63</v>
+      </c>
+      <c r="B2">
+        <v>3300</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>81</v>
+      </c>
+      <c r="B3">
+        <v>3650</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>88</v>
+      </c>
+      <c r="B4">
+        <v>3720</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>103.6</v>
+      </c>
+      <c r="B5">
+        <v>3900</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>112</v>
+      </c>
+      <c r="B6">
+        <v>4020</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A8">
+        <v>121</v>
+      </c>
+      <c r="B8">
+        <v>4060</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A10">
+        <v>129</v>
+      </c>
+      <c r="B10">
+        <v>4200</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A11">
+        <v>139.30000000000001</v>
+      </c>
+      <c r="B11">
+        <v>4510</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A12">
+        <v>142.6</v>
+      </c>
+      <c r="B12">
+        <v>4600</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A13">
+        <v>147.69999999999999</v>
+      </c>
+      <c r="B13">
+        <v>4700</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A14">
+        <v>183</v>
+      </c>
+      <c r="B14">
+        <v>5800</v>
       </c>
     </row>
   </sheetData>

</xml_diff>